<commit_message>
#61 Changed name of option from converter to fieldType
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/reader/TestBook_ValueConverter_Converted.xlsx
+++ b/src/test/resources/org/xlbean/reader/TestBook_ValueConverter_Converted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\src\test\resources\org\xlbean\reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8FE473-2A5E-4782-BA35-A82E6D692D71}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE377B9-D5E2-4F8D-9D7F-7B41C350B7BC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6252" yWindow="3684" windowWidth="21948" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="-108" windowWidth="29448" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="format" sheetId="3" r:id="rId1"/>
@@ -109,10 +109,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>testConverter?converter</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>bigdecimal</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -162,6 +158,10 @@
   </si>
   <si>
     <t>boolean</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>testConverter?fieldType</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -839,64 +839,64 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>29</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
         <v>30</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" t="s">
         <v>37</v>
       </c>
-      <c r="J3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="Q3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3" t="s">
         <v>33</v>
       </c>
-      <c r="M3" t="s">
+      <c r="U3" t="s">
         <v>34</v>
-      </c>
-      <c r="N3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" t="s">
-        <v>36</v>
-      </c>
-      <c r="P3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S3" t="s">
-        <v>37</v>
-      </c>
-      <c r="T3" t="s">
-        <v>34</v>
-      </c>
-      <c r="U3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.45">

</xml_diff>